<commit_message>
CHC identification for Flying/Not Flying experiment.
</commit_message>
<xml_diff>
--- a/data/raw/Flying/tmp/Ca-FALSE_RT_ID_table.xlsx
+++ b/data/raw/Flying/tmp/Ca-FALSE_RT_ID_table.xlsx
@@ -833,7 +833,7 @@
     <t xml:space="preserve">P216</t>
   </si>
   <si>
-    <t xml:space="preserve">C31_Me_11;13;15-</t>
+    <t xml:space="preserve">C31_Me_13;15-</t>
   </si>
   <si>
     <t xml:space="preserve">P217</t>
@@ -1044,12 +1044,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1145,14 +1141,14 @@
   <dimension ref="A1:M254"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B196" activeCellId="0" sqref="B196"/>
+      <selection pane="bottomLeft" activeCell="B222" activeCellId="0" sqref="B222"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2799,23 +2795,23 @@
         <v>20.719</v>
       </c>
     </row>
-    <row r="73" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
+    <row r="73" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="2" t="n">
+      <c r="C73" s="1" t="n">
         <v>20.962</v>
       </c>
-      <c r="D73" s="2" t="n">
+      <c r="D73" s="1" t="n">
         <v>20.995</v>
       </c>
-      <c r="E73" s="2" t="n">
+      <c r="E73" s="1" t="n">
         <v>20.953</v>
       </c>
-      <c r="F73" s="2" t="n">
+      <c r="F73" s="1" t="n">
         <v>20.96</v>
       </c>
-      <c r="J73" s="2" t="n">
+      <c r="J73" s="1" t="n">
         <v>20.94</v>
       </c>
     </row>
@@ -5153,7 +5149,7 @@
       <c r="A156" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C156" s="0" t="n">
@@ -5162,7 +5158,7 @@
       <c r="G156" s="0" t="n">
         <v>35.468</v>
       </c>
-      <c r="H156" s="4" t="n">
+      <c r="H156" s="3" t="n">
         <v>35.351</v>
       </c>
     </row>
@@ -5476,7 +5472,7 @@
       <c r="A166" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B166" s="3"/>
+      <c r="B166" s="2"/>
       <c r="C166" s="0" t="n">
         <v>36.9635555555556</v>
       </c>
@@ -5489,7 +5485,7 @@
       <c r="F166" s="0" t="n">
         <v>36.964</v>
       </c>
-      <c r="G166" s="3" t="n">
+      <c r="G166" s="2" t="n">
         <v>36.964</v>
       </c>
       <c r="H166" s="0" t="n">
@@ -5781,7 +5777,7 @@
       <c r="A177" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="B177" s="2" t="s">
         <v>210</v>
       </c>
       <c r="C177" s="0" t="n">
@@ -6842,7 +6838,7 @@
       <c r="A211" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="B211" s="3" t="s">
+      <c r="B211" s="2" t="s">
         <v>253</v>
       </c>
       <c r="C211" s="0" t="n">
@@ -7028,7 +7024,7 @@
       <c r="A217" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="B217" s="3" t="s">
+      <c r="B217" s="2" t="s">
         <v>262</v>
       </c>
       <c r="C217" s="0" t="n">
@@ -7303,7 +7299,7 @@
       <c r="A227" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="B227" s="3" t="s">
+      <c r="B227" s="2" t="s">
         <v>274</v>
       </c>
       <c r="C227" s="0" t="n">
@@ -7408,7 +7404,7 @@
       <c r="A230" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="B230" s="3" t="s">
+      <c r="B230" s="2" t="s">
         <v>279</v>
       </c>
       <c r="C230" s="0" t="n">

</xml_diff>

<commit_message>
Continued work on master table for Flying/Not Flying experiment along with sorting files in repository.
</commit_message>
<xml_diff>
--- a/data/raw/Flying/tmp/Ca-FALSE_RT_ID_table.xlsx
+++ b/data/raw/Flying/tmp/Ca-FALSE_RT_ID_table.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="H156" authorId="0">
+    <comment ref="B211" authorId="0">
       <text>
         <r>
           <rPr>
@@ -35,8 +35,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Not same compound
-</t>
+          <t xml:space="preserve">Fuse 210 &amp; 209</t>
         </r>
       </text>
     </comment>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="302">
   <si>
     <t xml:space="preserve">Peak</t>
   </si>
@@ -596,9 +595,6 @@
     <t xml:space="preserve">P155</t>
   </si>
   <si>
-    <t xml:space="preserve">C24_Me_2-</t>
-  </si>
-  <si>
     <t xml:space="preserve">P156</t>
   </si>
   <si>
@@ -675,9 +671,6 @@
   </si>
   <si>
     <t xml:space="preserve">P176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26_Me_2-</t>
   </si>
   <si>
     <t xml:space="preserve">P177</t>
@@ -990,7 +983,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,12 +994,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFA6"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA6A6"/>
-        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -1044,7 +1031,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1053,11 +1040,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1109,7 +1100,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFFA6A6"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -1141,12 +1132,12 @@
   <dimension ref="A1:M254"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B222" activeCellId="0" sqref="B222"/>
+      <selection pane="bottomLeft" activeCell="B217" activeCellId="0" sqref="B217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
   </cols>
@@ -5149,9 +5140,7 @@
       <c r="A156" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B156" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="B156" s="2"/>
       <c r="C156" s="0" t="n">
         <v>35.4095</v>
       </c>
@@ -5164,10 +5153,10 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B157" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="B157" s="0" t="s">
-        <v>185</v>
       </c>
       <c r="C157" s="0" t="n">
         <v>35.561</v>
@@ -5196,10 +5185,10 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B158" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="B158" s="0" t="s">
-        <v>187</v>
       </c>
       <c r="C158" s="0" t="n">
         <v>35.6385</v>
@@ -5237,10 +5226,10 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C159" s="0" t="n">
         <v>35.7362222222222</v>
@@ -5275,10 +5264,10 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B160" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="B160" s="0" t="s">
-        <v>190</v>
       </c>
       <c r="C160" s="0" t="n">
         <v>35.882</v>
@@ -5295,7 +5284,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C161" s="0" t="n">
         <v>36.146</v>
@@ -5333,7 +5322,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C162" s="0" t="n">
         <v>36.249125</v>
@@ -5365,7 +5354,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C163" s="0" t="n">
         <v>36.3675714285714</v>
@@ -5394,7 +5383,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C164" s="0" t="n">
         <v>36.5154</v>
@@ -5432,7 +5421,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C165" s="0" t="n">
         <v>36.7948</v>
@@ -5470,7 +5459,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" s="0" t="n">
@@ -5506,10 +5495,10 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B167" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="B167" s="0" t="s">
-        <v>198</v>
       </c>
       <c r="C167" s="0" t="n">
         <v>37.1253333333333</v>
@@ -5535,7 +5524,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C168" s="0" t="n">
         <v>37.2129</v>
@@ -5573,7 +5562,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C169" s="0" t="n">
         <v>37.358</v>
@@ -5584,10 +5573,10 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B170" s="0" t="s">
         <v>201</v>
-      </c>
-      <c r="B170" s="0" t="s">
-        <v>202</v>
       </c>
       <c r="C170" s="0" t="n">
         <v>37.5139</v>
@@ -5625,7 +5614,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C171" s="0" t="n">
         <v>37.709</v>
@@ -5636,7 +5625,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C172" s="0" t="n">
         <v>37.8806</v>
@@ -5659,7 +5648,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C173" s="0" t="n">
         <v>37.9941</v>
@@ -5697,7 +5686,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C174" s="0" t="n">
         <v>38.0942857142857</v>
@@ -5726,7 +5715,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>38.1745</v>
@@ -5758,7 +5747,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C176" s="0" t="n">
         <v>38.2703333333333</v>
@@ -5775,11 +5764,9 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>210</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B177" s="2"/>
       <c r="C177" s="0" t="n">
         <v>38.4223333333333</v>
       </c>
@@ -5813,10 +5800,10 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C178" s="0" t="n">
         <v>38.6057</v>
@@ -5854,10 +5841,10 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C179" s="0" t="n">
         <v>38.7083</v>
@@ -5895,7 +5882,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C180" s="0" t="n">
         <v>38.823</v>
@@ -5909,10 +5896,10 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C181" s="0" t="n">
         <v>39.06</v>
@@ -5950,7 +5937,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C182" s="0" t="n">
         <v>39.207125</v>
@@ -5982,10 +5969,10 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C183" s="0" t="n">
         <v>39.4156</v>
@@ -6023,7 +6010,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C184" s="0" t="n">
         <v>39.6518</v>
@@ -6061,7 +6048,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C185" s="0" t="n">
         <v>39.8137777777778</v>
@@ -6096,7 +6083,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C186" s="0" t="n">
         <v>39.9788333333333</v>
@@ -6122,7 +6109,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C187" s="0" t="n">
         <v>40.0672222222222</v>
@@ -6157,7 +6144,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C188" s="0" t="n">
         <v>40.143</v>
@@ -6168,7 +6155,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C189" s="0" t="n">
         <v>40.267</v>
@@ -6179,10 +6166,10 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C190" s="0" t="n">
         <v>40.3375</v>
@@ -6220,7 +6207,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C191" s="0" t="n">
         <v>40.631</v>
@@ -6240,7 +6227,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C192" s="0" t="n">
         <v>40.7584</v>
@@ -6278,7 +6265,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C193" s="0" t="n">
         <v>40.84675</v>
@@ -6298,7 +6285,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C194" s="0" t="n">
         <v>40.9959</v>
@@ -6336,7 +6323,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C195" s="0" t="n">
         <v>41.098</v>
@@ -6365,7 +6352,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C196" s="0" t="n">
         <v>41.1987</v>
@@ -6403,10 +6390,10 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C197" s="0" t="n">
         <v>41.3755</v>
@@ -6444,10 +6431,10 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C198" s="0" t="n">
         <v>41.438</v>
@@ -6467,10 +6454,10 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C199" s="0" t="n">
         <v>41.7306</v>
@@ -6508,7 +6495,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C200" s="0" t="n">
         <v>41.9465</v>
@@ -6528,10 +6515,10 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C201" s="0" t="n">
         <v>42.0894</v>
@@ -6569,7 +6556,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C202" s="0" t="n">
         <v>42.343</v>
@@ -6580,7 +6567,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C203" s="0" t="n">
         <v>42.4677</v>
@@ -6618,7 +6605,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C204" s="0" t="n">
         <v>42.6947777777778</v>
@@ -6653,7 +6640,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C205" s="0" t="n">
         <v>42.8579</v>
@@ -6691,10 +6678,10 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C206" s="0" t="n">
         <v>42.9756</v>
@@ -6732,7 +6719,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C207" s="0" t="n">
         <v>43.1735</v>
@@ -6746,7 +6733,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C208" s="0" t="n">
         <v>43.361</v>
@@ -6781,7 +6768,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C209" s="0" t="n">
         <v>43.504</v>
@@ -6810,7 +6797,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C210" s="0" t="n">
         <v>43.6401666666667</v>
@@ -6836,10 +6823,10 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="C211" s="0" t="n">
         <v>43.7318</v>
@@ -6877,10 +6864,10 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C212" s="0" t="n">
         <v>43.9442</v>
@@ -6918,10 +6905,10 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C213" s="0" t="n">
         <v>44.0334</v>
@@ -6959,7 +6946,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C214" s="0" t="n">
         <v>44.129</v>
@@ -6970,10 +6957,10 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C215" s="0" t="n">
         <v>44.2627</v>
@@ -7011,7 +6998,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C216" s="0" t="n">
         <v>44.522</v>
@@ -7022,10 +7009,10 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>260</v>
       </c>
       <c r="C217" s="0" t="n">
         <v>44.6054</v>
@@ -7063,7 +7050,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C218" s="0" t="n">
         <v>44.708</v>
@@ -7077,7 +7064,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C219" s="0" t="n">
         <v>44.8735</v>
@@ -7091,7 +7078,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C220" s="0" t="n">
         <v>44.932375</v>
@@ -7123,7 +7110,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C221" s="0" t="n">
         <v>45.005</v>
@@ -7134,10 +7121,10 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C222" s="0" t="n">
         <v>45.1915</v>
@@ -7175,7 +7162,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C223" s="0" t="n">
         <v>45.33875</v>
@@ -7195,7 +7182,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C224" s="0" t="n">
         <v>45.4076</v>
@@ -7233,7 +7220,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C225" s="0" t="n">
         <v>45.623</v>
@@ -7271,7 +7258,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C226" s="0" t="n">
         <v>45.8138333333333</v>
@@ -7297,10 +7284,10 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="C227" s="0" t="n">
         <v>46.1237</v>
@@ -7338,10 +7325,10 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C228" s="0" t="n">
         <v>46.3932</v>
@@ -7379,7 +7366,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C229" s="0" t="n">
         <v>46.4702</v>
@@ -7402,10 +7389,10 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="C230" s="0" t="n">
         <v>46.6404</v>
@@ -7443,7 +7430,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C231" s="0" t="n">
         <v>46.7943</v>
@@ -7481,7 +7468,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C232" s="0" t="n">
         <v>47.011</v>
@@ -7516,7 +7503,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C233" s="0" t="n">
         <v>47.135</v>
@@ -7539,7 +7526,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C234" s="0" t="n">
         <v>47.2522222222222</v>
@@ -7574,7 +7561,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C235" s="0" t="n">
         <v>47.4353333333333</v>
@@ -7609,7 +7596,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C236" s="0" t="n">
         <v>47.6648333333333</v>
@@ -7635,7 +7622,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C237" s="0" t="n">
         <v>47.7915555555556</v>
@@ -7670,7 +7657,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C238" s="0" t="n">
         <v>48.3761</v>
@@ -7708,7 +7695,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C239" s="0" t="n">
         <v>48.5892222222222</v>
@@ -7743,7 +7730,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C240" s="0" t="n">
         <v>48.8544444444444</v>
@@ -7778,7 +7765,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C241" s="0" t="n">
         <v>49.214</v>
@@ -7792,7 +7779,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C242" s="0" t="n">
         <v>49.8874285714286</v>
@@ -7821,7 +7808,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C243" s="0" t="n">
         <v>50.0203333333333</v>
@@ -7856,7 +7843,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C244" s="0" t="n">
         <v>50.7555</v>
@@ -7882,7 +7869,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C245" s="0" t="n">
         <v>51.4275</v>
@@ -7896,7 +7883,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C246" s="0" t="n">
         <v>52.1557777777778</v>
@@ -7931,7 +7918,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C247" s="0" t="n">
         <v>52.51</v>
@@ -7945,7 +7932,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C248" s="0" t="n">
         <v>52.741</v>
@@ -7956,7 +7943,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C249" s="0" t="n">
         <v>53.723</v>
@@ -7979,7 +7966,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C250" s="0" t="n">
         <v>55.148</v>
@@ -7990,7 +7977,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C251" s="0" t="n">
         <v>55.8338888888889</v>
@@ -8025,7 +8012,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C252" s="0" t="n">
         <v>56.43</v>
@@ -8051,7 +8038,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C253" s="0" t="n">
         <v>56.685</v>
@@ -8062,7 +8049,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C254" s="0" t="n">
         <v>57.5885</v>

</xml_diff>